<commit_message>
Adding research doc for cloud resource data
</commit_message>
<xml_diff>
--- a/resources/documents/VM results.xlsx
+++ b/resources/documents/VM results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Microwave\outlier-detection-in-virtual-machines\resources\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11140ADF-1DEB-4ADE-A601-ED71A958262C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CB68E2-0CFA-4C15-96D2-E45500DBD40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="6210" windowWidth="12060" windowHeight="7260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6435" yWindow="5805" windowWidth="10845" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -444,7 +444,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>90</v>
+        <v>99.97</v>
       </c>
       <c r="E2">
         <v>50</v>
@@ -550,16 +550,16 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>56.2</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="E3">
         <v>100</v>
       </c>
       <c r="F3">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="G3">
-        <v>0.3</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H3">
         <v>21.632300000000001</v>
@@ -591,16 +591,16 @@
         <v>8</v>
       </c>
       <c r="D4">
-        <v>33.299999999999997</v>
+        <v>43.23</v>
       </c>
       <c r="E4">
         <v>100</v>
       </c>
       <c r="F4">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="G4">
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
       <c r="H4">
         <v>25.660699999999999</v>
@@ -632,7 +632,7 @@
         <v>10</v>
       </c>
       <c r="D5">
-        <v>89.2</v>
+        <v>99.2</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -673,7 +673,7 @@
         <v>12</v>
       </c>
       <c r="D6">
-        <v>91.4</v>
+        <v>99.9</v>
       </c>
       <c r="E6">
         <v>50</v>
@@ -682,7 +682,7 @@
         <v>20</v>
       </c>
       <c r="G6">
-        <v>28.6</v>
+        <v>28.57</v>
       </c>
       <c r="H6">
         <v>14.4061</v>
@@ -714,7 +714,7 @@
         <v>14</v>
       </c>
       <c r="D7">
-        <v>90</v>
+        <v>99.98</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -755,7 +755,7 @@
         <v>16</v>
       </c>
       <c r="D8">
-        <v>70.3</v>
+        <v>70.260000000000005</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -796,7 +796,7 @@
         <v>18</v>
       </c>
       <c r="D9">
-        <v>90.1</v>
+        <v>100</v>
       </c>
       <c r="E9">
         <v>50</v>
@@ -805,7 +805,7 @@
         <v>100</v>
       </c>
       <c r="G9">
-        <v>66.7</v>
+        <v>66.67</v>
       </c>
       <c r="H9">
         <v>13.734</v>
@@ -837,7 +837,7 @@
         <v>20</v>
       </c>
       <c r="D10">
-        <v>90</v>
+        <v>99.98</v>
       </c>
       <c r="E10">
         <v>50</v>
@@ -873,7 +873,7 @@
       </c>
       <c r="D11">
         <f t="shared" ref="D11" si="0">AVERAGE(D2:D10)</f>
-        <v>77.833333333333329</v>
+        <v>86.513333333333335</v>
       </c>
       <c r="E11">
         <f>AVERAGE(E2:E7,E9,E10)</f>
@@ -881,11 +881,11 @@
       </c>
       <c r="F11">
         <f t="shared" ref="F11:G11" si="1">AVERAGE(F2:F7,F9,F10)</f>
-        <v>27.524999999999999</v>
+        <v>27.53</v>
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
-        <v>24.475000000000001</v>
+        <v>24.462499999999999</v>
       </c>
       <c r="H11">
         <f>AVERAGE(H2:H10)</f>
@@ -948,7 +948,7 @@
         <v>4</v>
       </c>
       <c r="D16">
-        <v>90</v>
+        <v>99.98</v>
       </c>
       <c r="E16">
         <v>50</v>
@@ -974,16 +974,16 @@
         <v>6</v>
       </c>
       <c r="D17">
-        <v>67.8</v>
+        <v>77.75</v>
       </c>
       <c r="E17">
         <v>100</v>
       </c>
       <c r="F17">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="G17">
-        <v>0.4</v>
+        <v>0.44</v>
       </c>
       <c r="H17">
         <v>7.2271000000000001</v>
@@ -1000,16 +1000,16 @@
         <v>8</v>
       </c>
       <c r="D18">
-        <v>68.3</v>
+        <v>78.17</v>
       </c>
       <c r="E18">
         <v>100</v>
       </c>
       <c r="F18">
-        <v>0.2</v>
+        <v>0.23</v>
       </c>
       <c r="G18">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="H18">
         <v>8.7147000000000006</v>
@@ -1026,7 +1026,7 @@
         <v>10</v>
       </c>
       <c r="D19">
-        <v>89.9</v>
+        <v>99.93</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1052,13 +1052,13 @@
         <v>12</v>
       </c>
       <c r="D20">
-        <v>91.4</v>
+        <v>99.88</v>
       </c>
       <c r="E20">
         <v>50</v>
       </c>
       <c r="F20">
-        <v>16.7</v>
+        <v>16.670000000000002</v>
       </c>
       <c r="G20">
         <v>25</v>
@@ -1078,7 +1078,7 @@
         <v>14</v>
       </c>
       <c r="D21">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1104,7 +1104,7 @@
         <v>16</v>
       </c>
       <c r="D22">
-        <v>76.8</v>
+        <v>76.81</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1130,7 +1130,7 @@
         <v>18</v>
       </c>
       <c r="D23">
-        <v>90.1</v>
+        <v>100</v>
       </c>
       <c r="E23">
         <v>50</v>
@@ -1139,7 +1139,7 @@
         <v>100</v>
       </c>
       <c r="G23">
-        <v>66.7</v>
+        <v>66.67</v>
       </c>
       <c r="H23">
         <v>5.0815999999999999</v>
@@ -1156,16 +1156,16 @@
         <v>20</v>
       </c>
       <c r="D24">
-        <v>89.9</v>
+        <v>99.85</v>
       </c>
       <c r="E24">
         <v>50</v>
       </c>
       <c r="F24">
-        <v>14.3</v>
+        <v>14.29</v>
       </c>
       <c r="G24">
-        <v>22.2</v>
+        <v>22.22</v>
       </c>
       <c r="H24">
         <v>6.8909000000000002</v>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="D25">
         <f>AVERAGE(D16:D24)</f>
-        <v>83.8</v>
+        <v>92.48555555555555</v>
       </c>
       <c r="E25">
         <f t="shared" ref="E25:H25" si="3">AVERAGE(E16:E24)</f>
@@ -1185,11 +1185,11 @@
       </c>
       <c r="F25">
         <f t="shared" si="3"/>
-        <v>20.155555555555559</v>
+        <v>20.156666666666666</v>
       </c>
       <c r="G25">
         <f t="shared" si="3"/>
-        <v>18.311111111111114</v>
+        <v>18.308888888888887</v>
       </c>
       <c r="H25">
         <f t="shared" si="3"/>

</xml_diff>